<commit_message>
lainnya and login ui
</commit_message>
<xml_diff>
--- a/public/template-import-excel/edom-excel-import-dosen.xlsx
+++ b/public/template-import-excel/edom-excel-import-dosen.xlsx
@@ -16,17 +16,6 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
-  <si>
-    <t>Nama Dosen</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -121,7 +110,7 @@
   <cols>
     <col min="1" max="1" style="1" width="9.142307692307693"/>
     <col min="2" max="2" style="1" width="32.42662259615385" customWidth="1"/>
-    <col min="3" max="3" style="1" width="26.71268028846154" customWidth="1"/>
+    <col min="3" max="3" style="1" width="52.42542067307693" customWidth="1"/>
     <col min="4" max="4" style="1" width="34.42650240384616" customWidth="1"/>
     <col min="5" max="5" style="1" width="10.999338942307693" customWidth="1"/>
     <col min="6" max="16384" style="1" width="9.142307692307693"/>
@@ -138,11 +127,15 @@
           <t>NIP NPAK atau NIDN</t>
         </is>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Nama Dosen</t>
+        </is>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>

</xml_diff>